<commit_message>
I2C_SetFrequency() function added, default is 57.6Khz, 3 options in i2c.h
</commit_message>
<xml_diff>
--- a/scratch/i2ctest/I2C_CCR clock settings.xlsx
+++ b/scratch/i2ctest/I2C_CCR clock settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\Agon\scratch\i2ctest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A276D03-F3C5-4484-923B-F8BC4ED7EFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DFF983-1DF5-44A9-82DB-1F5CCF0413F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BEBEE3E6-138F-40F9-957C-D0853634FDFA}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{BEBEE3E6-138F-40F9-957C-D0853634FDFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>